<commit_message>
updates for CR11 preparation
</commit_message>
<xml_diff>
--- a/publication/part1000/CR00011/CR11_WG_Numbers_table.xlsx
+++ b/publication/part1000/CR00011/CR11_WG_Numbers_table.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1056" uniqueCount="702">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1059" uniqueCount="704">
   <si>
     <t>N8573</t>
   </si>
@@ -1071,12 +1071,6 @@
     <t>ISO 10303-1601  ed  4 altered_package Document</t>
   </si>
   <si>
-    <t>ISO 10303-1765  ed  4 characterizable_object Document</t>
-  </si>
-  <si>
-    <t>ISO 10303-1765  ed  4 characterizable_object ARM EXPRESS</t>
-  </si>
-  <si>
     <t>ISO 10303-409  ed  2 ap209_multidisciplinary_analysis_and_design Document</t>
   </si>
   <si>
@@ -1245,18 +1239,6 @@
     <t>ISO 10303-1649  ed  5 assembly_technology MIM EXPRESS</t>
   </si>
   <si>
-    <t>ISO 10303-1808  ed  3 assembly_shape Document</t>
-  </si>
-  <si>
-    <t>ISO 10303-1808  ed  3 assembly_shape ARM EXPRESS</t>
-  </si>
-  <si>
-    <t>ISO 10303-1026  ed  6 assembly_structure Document</t>
-  </si>
-  <si>
-    <t>ISO 10303-1026  ed  6 assembly_structure ARM EXPRESS</t>
-  </si>
-  <si>
     <t>ISO 10303-1311  ed  5 associative_draughting_elements Document</t>
   </si>
   <si>
@@ -2125,6 +2107,30 @@
   </si>
   <si>
     <t>ISO 10303-1819  ed  2 tessellated_geometry ARM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1808  ed  2 assembly_shape Document</t>
+  </si>
+  <si>
+    <t>ISO 10303-1808  ed  2 assembly_shape ARM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1026  ed  5 assembly_structure Document</t>
+  </si>
+  <si>
+    <t>ISO 10303-1026  ed  5 assembly_structure ARM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1765  ed  3 characterizable_object Document</t>
+  </si>
+  <si>
+    <t>ISO 10303-1765  ed  3 characterizable_object ARM EXPRESS</t>
+  </si>
+  <si>
+    <t>N9123</t>
+  </si>
+  <si>
+    <t>ISO 10303-1662  ed  4 design_specific_assignment_to_assembly_usage_view ARM EXPRESS</t>
   </si>
 </sst>
 </file>
@@ -2194,8 +2200,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="767">
+  <cellStyleXfs count="777">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2979,7 +2995,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="767">
+  <cellStyles count="777">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
@@ -3363,6 +3379,11 @@
     <cellStyle name="Lien hypertexte" xfId="761" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="763" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="765" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="767" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="769" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="771" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="773" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="775" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
@@ -3746,6 +3767,11 @@
     <cellStyle name="Lien hypertexte visité" xfId="762" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="764" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="766" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="768" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="770" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="772" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="774" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="776" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4075,10 +4101,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F352"/>
+  <dimension ref="A1:F353"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
-      <selection activeCell="E133" sqref="E133"/>
+    <sheetView tabSelected="1" topLeftCell="A330" workbookViewId="0">
+      <selection activeCell="B353" sqref="B353:D353"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4086,6 +4112,7 @@
     <col min="2" max="2" width="15.5" customWidth="1"/>
     <col min="3" max="4" width="10.5" customWidth="1"/>
     <col min="5" max="5" width="70.6640625" customWidth="1"/>
+    <col min="6" max="6" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -4178,7 +4205,7 @@
       <c r="C6" s="1"/>
       <c r="D6" s="2"/>
       <c r="E6" s="3" t="s">
-        <v>350</v>
+        <v>700</v>
       </c>
       <c r="F6" s="4">
         <v>42013</v>
@@ -4194,7 +4221,7 @@
       <c r="C7" s="1"/>
       <c r="D7" s="2"/>
       <c r="E7" s="3" t="s">
-        <v>351</v>
+        <v>701</v>
       </c>
       <c r="F7" s="4">
         <v>42013</v>
@@ -4210,7 +4237,7 @@
       <c r="C8" s="1"/>
       <c r="D8" s="2"/>
       <c r="E8" s="3" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="F8" s="4">
         <v>42013</v>
@@ -4226,7 +4253,7 @@
       <c r="C9" s="1"/>
       <c r="D9" s="2"/>
       <c r="E9" s="3" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="F9" s="4">
         <v>42013</v>
@@ -4242,7 +4269,7 @@
       <c r="C10" s="1"/>
       <c r="D10" s="2"/>
       <c r="E10" s="3" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="F10" s="4">
         <v>42013</v>
@@ -4258,7 +4285,7 @@
       <c r="C11" s="1"/>
       <c r="D11" s="2"/>
       <c r="E11" s="3" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="F11" s="4">
         <v>42013</v>
@@ -4274,7 +4301,7 @@
       <c r="C12" s="1"/>
       <c r="D12" s="2"/>
       <c r="E12" s="3" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="F12" s="4">
         <v>42013</v>
@@ -4290,7 +4317,7 @@
       <c r="C13" s="1"/>
       <c r="D13" s="2"/>
       <c r="E13" s="3" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="F13" s="4">
         <v>42013</v>
@@ -4306,7 +4333,7 @@
       <c r="C14" s="1"/>
       <c r="D14" s="2"/>
       <c r="E14" s="3" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="F14" s="4">
         <v>42013</v>
@@ -4322,7 +4349,7 @@
       <c r="C15" s="1"/>
       <c r="D15" s="2"/>
       <c r="E15" s="3" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="F15" s="4">
         <v>42013</v>
@@ -4338,7 +4365,7 @@
       <c r="C16" s="1"/>
       <c r="D16" s="2"/>
       <c r="E16" s="3" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="F16" s="4">
         <v>42013</v>
@@ -4354,7 +4381,7 @@
       <c r="C17" s="1"/>
       <c r="D17" s="2"/>
       <c r="E17" s="3" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="F17" s="4">
         <v>42013</v>
@@ -4370,7 +4397,7 @@
       <c r="C18" s="1"/>
       <c r="D18" s="2"/>
       <c r="E18" s="3" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="F18" s="4">
         <v>42013</v>
@@ -4386,7 +4413,7 @@
       <c r="C19" s="1"/>
       <c r="D19" s="2"/>
       <c r="E19" s="3" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="F19" s="4">
         <v>42013</v>
@@ -4402,7 +4429,7 @@
       <c r="C20" s="1"/>
       <c r="D20" s="2"/>
       <c r="E20" s="3" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="F20" s="4">
         <v>42013</v>
@@ -4418,7 +4445,7 @@
       <c r="C21" s="1"/>
       <c r="D21" s="2"/>
       <c r="E21" s="3" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="F21" s="4">
         <v>42013</v>
@@ -4434,7 +4461,7 @@
       <c r="C22" s="1"/>
       <c r="D22" s="2"/>
       <c r="E22" s="3" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="F22" s="4">
         <v>42013</v>
@@ -4450,7 +4477,7 @@
       <c r="C23" s="1"/>
       <c r="D23" s="2"/>
       <c r="E23" s="3" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="F23" s="4">
         <v>42013</v>
@@ -4466,7 +4493,7 @@
       <c r="C24" s="1"/>
       <c r="D24" s="2"/>
       <c r="E24" s="3" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="F24" s="4">
         <v>42013</v>
@@ -4482,7 +4509,7 @@
       <c r="C25" s="1"/>
       <c r="D25" s="2"/>
       <c r="E25" s="3" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="F25" s="4">
         <v>42013</v>
@@ -4498,7 +4525,7 @@
       <c r="C26" s="1"/>
       <c r="D26" s="2"/>
       <c r="E26" s="3" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="F26" s="4">
         <v>42013</v>
@@ -4514,7 +4541,7 @@
       <c r="C27" s="1"/>
       <c r="D27" s="2"/>
       <c r="E27" s="3" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="F27" s="4">
         <v>42013</v>
@@ -4530,7 +4557,7 @@
       <c r="C28" s="1"/>
       <c r="D28" s="2"/>
       <c r="E28" s="3" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="F28" s="4">
         <v>42013</v>
@@ -4546,7 +4573,7 @@
       <c r="C29" s="1"/>
       <c r="D29" s="2"/>
       <c r="E29" s="3" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="F29" s="4">
         <v>42013</v>
@@ -4562,7 +4589,7 @@
       <c r="C30" s="1"/>
       <c r="D30" s="2"/>
       <c r="E30" s="3" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="F30" s="4">
         <v>42013</v>
@@ -4578,7 +4605,7 @@
       <c r="C31" s="1"/>
       <c r="D31" s="2"/>
       <c r="E31" s="3" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="F31" s="4">
         <v>42013</v>
@@ -4594,7 +4621,7 @@
       <c r="C32" s="1"/>
       <c r="D32" s="2"/>
       <c r="E32" s="3" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="F32" s="4">
         <v>42013</v>
@@ -4610,7 +4637,7 @@
       <c r="C33" s="1"/>
       <c r="D33" s="2"/>
       <c r="E33" s="3" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="F33" s="4">
         <v>42013</v>
@@ -4626,7 +4653,7 @@
       <c r="C34" s="1"/>
       <c r="D34" s="2"/>
       <c r="E34" s="3" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="F34" s="4">
         <v>42013</v>
@@ -4642,7 +4669,7 @@
       <c r="C35" s="1"/>
       <c r="D35" s="2"/>
       <c r="E35" s="3" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="F35" s="4">
         <v>42013</v>
@@ -4658,7 +4685,7 @@
       <c r="C36" s="1"/>
       <c r="D36" s="2"/>
       <c r="E36" s="3" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="F36" s="4">
         <v>42013</v>
@@ -4674,7 +4701,7 @@
       <c r="C37" s="1"/>
       <c r="D37" s="2"/>
       <c r="E37" s="3" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="F37" s="4">
         <v>42013</v>
@@ -4690,7 +4717,7 @@
       <c r="C38" s="1"/>
       <c r="D38" s="2"/>
       <c r="E38" s="3" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="F38" s="4">
         <v>42013</v>
@@ -4706,7 +4733,7 @@
       <c r="C39" s="1"/>
       <c r="D39" s="2"/>
       <c r="E39" s="3" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="F39" s="4">
         <v>42013</v>
@@ -4722,7 +4749,7 @@
       <c r="C40" s="1"/>
       <c r="D40" s="2"/>
       <c r="E40" s="3" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="F40" s="4">
         <v>42013</v>
@@ -4738,7 +4765,7 @@
       <c r="C41" s="1"/>
       <c r="D41" s="2"/>
       <c r="E41" s="3" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="F41" s="4">
         <v>42013</v>
@@ -4754,7 +4781,7 @@
       <c r="C42" s="1"/>
       <c r="D42" s="2"/>
       <c r="E42" s="3" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="F42" s="4">
         <v>42013</v>
@@ -4770,7 +4797,7 @@
       <c r="C43" s="1"/>
       <c r="D43" s="2"/>
       <c r="E43" s="3" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="F43" s="4">
         <v>42013</v>
@@ -4786,7 +4813,7 @@
       <c r="C44" s="1"/>
       <c r="D44" s="2"/>
       <c r="E44" s="3" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="F44" s="4">
         <v>42013</v>
@@ -4802,7 +4829,7 @@
       <c r="C45" s="1"/>
       <c r="D45" s="2"/>
       <c r="E45" s="3" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="F45" s="4">
         <v>42013</v>
@@ -4818,7 +4845,7 @@
       <c r="C46" s="1"/>
       <c r="D46" s="2"/>
       <c r="E46" s="3" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="F46" s="4">
         <v>42013</v>
@@ -4834,7 +4861,7 @@
       <c r="C47" s="1"/>
       <c r="D47" s="2"/>
       <c r="E47" s="3" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="F47" s="4">
         <v>42013</v>
@@ -4850,7 +4877,7 @@
       <c r="C48" s="1"/>
       <c r="D48" s="2"/>
       <c r="E48" s="3" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="F48" s="4">
         <v>42013</v>
@@ -4866,7 +4893,7 @@
       <c r="C49" s="1"/>
       <c r="D49" s="2"/>
       <c r="E49" s="3" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="F49" s="4">
         <v>42013</v>
@@ -4882,7 +4909,7 @@
       <c r="C50" s="1"/>
       <c r="D50" s="2"/>
       <c r="E50" s="3" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F50" s="4">
         <v>42013</v>
@@ -4898,7 +4925,7 @@
       <c r="C51" s="1"/>
       <c r="D51" s="2"/>
       <c r="E51" s="3" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="F51" s="4">
         <v>42013</v>
@@ -4914,7 +4941,7 @@
       <c r="C52" s="1"/>
       <c r="D52" s="2"/>
       <c r="E52" s="3" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="F52" s="4">
         <v>42013</v>
@@ -4930,7 +4957,7 @@
       <c r="C53" s="1"/>
       <c r="D53" s="2"/>
       <c r="E53" s="3" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="F53" s="4">
         <v>42013</v>
@@ -4946,7 +4973,7 @@
       <c r="C54" s="1"/>
       <c r="D54" s="2"/>
       <c r="E54" s="3" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="F54" s="4">
         <v>42013</v>
@@ -4962,7 +4989,7 @@
       <c r="C55" s="1"/>
       <c r="D55" s="2"/>
       <c r="E55" s="3" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="F55" s="4">
         <v>42013</v>
@@ -4978,7 +5005,7 @@
       <c r="C56" s="1"/>
       <c r="D56" s="2"/>
       <c r="E56" s="3" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="F56" s="4">
         <v>42013</v>
@@ -4994,7 +5021,7 @@
       <c r="C57" s="1"/>
       <c r="D57" s="2"/>
       <c r="E57" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="F57" s="4">
         <v>42013</v>
@@ -5010,7 +5037,7 @@
       <c r="C58" s="1"/>
       <c r="D58" s="2"/>
       <c r="E58" s="3" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="F58" s="4">
         <v>42013</v>
@@ -5026,7 +5053,7 @@
       <c r="C59" s="1"/>
       <c r="D59" s="2"/>
       <c r="E59" s="3" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="F59" s="4">
         <v>42013</v>
@@ -5042,7 +5069,7 @@
       <c r="C60" s="1"/>
       <c r="D60" s="2"/>
       <c r="E60" s="3" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="F60" s="4">
         <v>42013</v>
@@ -5058,7 +5085,7 @@
       <c r="C61" s="1"/>
       <c r="D61" s="2"/>
       <c r="E61" s="3" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="F61" s="4">
         <v>42013</v>
@@ -5074,7 +5101,7 @@
       <c r="C62" s="1"/>
       <c r="D62" s="2"/>
       <c r="E62" s="3" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="F62" s="4">
         <v>42013</v>
@@ -5090,7 +5117,7 @@
       <c r="C63" s="1"/>
       <c r="D63" s="2"/>
       <c r="E63" s="3" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="F63" s="4">
         <v>42013</v>
@@ -5106,7 +5133,7 @@
       <c r="C64" s="1"/>
       <c r="D64" s="2"/>
       <c r="E64" s="3" t="s">
-        <v>408</v>
+        <v>696</v>
       </c>
       <c r="F64" s="4">
         <v>42013</v>
@@ -5122,7 +5149,7 @@
       <c r="C65" s="1"/>
       <c r="D65" s="2"/>
       <c r="E65" s="3" t="s">
-        <v>409</v>
+        <v>697</v>
       </c>
       <c r="F65" s="4">
         <v>42013</v>
@@ -5138,7 +5165,7 @@
       <c r="C66" s="1"/>
       <c r="D66" s="2"/>
       <c r="E66" s="3" t="s">
-        <v>410</v>
+        <v>698</v>
       </c>
       <c r="F66" s="4">
         <v>42013</v>
@@ -5154,7 +5181,7 @@
       <c r="C67" s="1"/>
       <c r="D67" s="2"/>
       <c r="E67" s="3" t="s">
-        <v>411</v>
+        <v>699</v>
       </c>
       <c r="F67" s="4">
         <v>42013</v>
@@ -5170,7 +5197,7 @@
       <c r="C68" s="1"/>
       <c r="D68" s="2"/>
       <c r="E68" s="3" t="s">
-        <v>412</v>
+        <v>406</v>
       </c>
       <c r="F68" s="4">
         <v>42013</v>
@@ -5186,7 +5213,7 @@
       <c r="C69" s="1"/>
       <c r="D69" s="2"/>
       <c r="E69" s="3" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="F69" s="4">
         <v>42013</v>
@@ -5202,7 +5229,7 @@
       <c r="C70" s="1"/>
       <c r="D70" s="2"/>
       <c r="E70" s="3" t="s">
-        <v>414</v>
+        <v>408</v>
       </c>
       <c r="F70" s="4">
         <v>42013</v>
@@ -5218,7 +5245,7 @@
       <c r="C71" s="1"/>
       <c r="D71" s="2"/>
       <c r="E71" s="3" t="s">
-        <v>415</v>
+        <v>409</v>
       </c>
       <c r="F71" s="4">
         <v>42013</v>
@@ -5234,7 +5261,7 @@
       <c r="C72" s="1"/>
       <c r="D72" s="2"/>
       <c r="E72" s="3" t="s">
-        <v>416</v>
+        <v>410</v>
       </c>
       <c r="F72" s="4">
         <v>42013</v>
@@ -5250,7 +5277,7 @@
       <c r="C73" s="1"/>
       <c r="D73" s="2"/>
       <c r="E73" s="3" t="s">
-        <v>417</v>
+        <v>411</v>
       </c>
       <c r="F73" s="4">
         <v>42013</v>
@@ -5266,7 +5293,7 @@
       <c r="C74" s="1"/>
       <c r="D74" s="2"/>
       <c r="E74" s="3" t="s">
-        <v>418</v>
+        <v>412</v>
       </c>
       <c r="F74" s="4">
         <v>42013</v>
@@ -5282,7 +5309,7 @@
       <c r="C75" s="1"/>
       <c r="D75" s="2"/>
       <c r="E75" s="3" t="s">
-        <v>419</v>
+        <v>413</v>
       </c>
       <c r="F75" s="4">
         <v>42013</v>
@@ -5298,7 +5325,7 @@
       <c r="C76" s="1"/>
       <c r="D76" s="2"/>
       <c r="E76" s="3" t="s">
-        <v>420</v>
+        <v>414</v>
       </c>
       <c r="F76" s="4">
         <v>42013</v>
@@ -5314,7 +5341,7 @@
       <c r="C77" s="1"/>
       <c r="D77" s="2"/>
       <c r="E77" s="3" t="s">
-        <v>421</v>
+        <v>415</v>
       </c>
       <c r="F77" s="4">
         <v>42013</v>
@@ -5330,7 +5357,7 @@
       <c r="C78" s="1"/>
       <c r="D78" s="2"/>
       <c r="E78" s="3" t="s">
-        <v>422</v>
+        <v>416</v>
       </c>
       <c r="F78" s="4">
         <v>42013</v>
@@ -5346,7 +5373,7 @@
       <c r="C79" s="1"/>
       <c r="D79" s="2"/>
       <c r="E79" s="3" t="s">
-        <v>423</v>
+        <v>417</v>
       </c>
       <c r="F79" s="4">
         <v>42013</v>
@@ -5362,7 +5389,7 @@
       <c r="C80" s="1"/>
       <c r="D80" s="2"/>
       <c r="E80" s="3" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
       <c r="F80" s="4">
         <v>42013</v>
@@ -5378,7 +5405,7 @@
       <c r="C81" s="1"/>
       <c r="D81" s="2"/>
       <c r="E81" s="3" t="s">
-        <v>425</v>
+        <v>419</v>
       </c>
       <c r="F81" s="4">
         <v>42013</v>
@@ -5394,7 +5421,7 @@
       <c r="C82" s="1"/>
       <c r="D82" s="2"/>
       <c r="E82" s="3" t="s">
-        <v>426</v>
+        <v>420</v>
       </c>
       <c r="F82" s="4">
         <v>42013</v>
@@ -5410,7 +5437,7 @@
       <c r="C83" s="1"/>
       <c r="D83" s="2"/>
       <c r="E83" s="3" t="s">
-        <v>427</v>
+        <v>421</v>
       </c>
       <c r="F83" s="4">
         <v>42013</v>
@@ -5426,7 +5453,7 @@
       <c r="C84" s="1"/>
       <c r="D84" s="2"/>
       <c r="E84" s="3" t="s">
-        <v>428</v>
+        <v>422</v>
       </c>
       <c r="F84" s="4">
         <v>42013</v>
@@ -5442,7 +5469,7 @@
       <c r="C85" s="1"/>
       <c r="D85" s="2"/>
       <c r="E85" s="3" t="s">
-        <v>429</v>
+        <v>423</v>
       </c>
       <c r="F85" s="4">
         <v>42013</v>
@@ -5458,7 +5485,7 @@
       <c r="C86" s="1"/>
       <c r="D86" s="2"/>
       <c r="E86" s="3" t="s">
-        <v>430</v>
+        <v>424</v>
       </c>
       <c r="F86" s="4">
         <v>42013</v>
@@ -5474,7 +5501,7 @@
       <c r="C87" s="1"/>
       <c r="D87" s="2"/>
       <c r="E87" s="3" t="s">
-        <v>431</v>
+        <v>425</v>
       </c>
       <c r="F87" s="4">
         <v>42013</v>
@@ -5490,7 +5517,7 @@
       <c r="C88" s="1"/>
       <c r="D88" s="2"/>
       <c r="E88" s="3" t="s">
-        <v>432</v>
+        <v>426</v>
       </c>
       <c r="F88" s="4">
         <v>42013</v>
@@ -5506,7 +5533,7 @@
       <c r="C89" s="1"/>
       <c r="D89" s="2"/>
       <c r="E89" s="3" t="s">
-        <v>433</v>
+        <v>427</v>
       </c>
       <c r="F89" s="4">
         <v>42013</v>
@@ -5522,7 +5549,7 @@
       <c r="C90" s="1"/>
       <c r="D90" s="2"/>
       <c r="E90" s="3" t="s">
-        <v>434</v>
+        <v>428</v>
       </c>
       <c r="F90" s="4">
         <v>42013</v>
@@ -5538,7 +5565,7 @@
       <c r="C91" s="1"/>
       <c r="D91" s="2"/>
       <c r="E91" s="3" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
       <c r="F91" s="4">
         <v>42013</v>
@@ -5554,7 +5581,7 @@
       <c r="C92" s="1"/>
       <c r="D92" s="2"/>
       <c r="E92" s="3" t="s">
-        <v>436</v>
+        <v>430</v>
       </c>
       <c r="F92" s="4">
         <v>42013</v>
@@ -5570,7 +5597,7 @@
       <c r="C93" s="1"/>
       <c r="D93" s="2"/>
       <c r="E93" s="3" t="s">
-        <v>437</v>
+        <v>431</v>
       </c>
       <c r="F93" s="4">
         <v>42013</v>
@@ -5586,7 +5613,7 @@
       <c r="C94" s="1"/>
       <c r="D94" s="2"/>
       <c r="E94" s="3" t="s">
-        <v>438</v>
+        <v>432</v>
       </c>
       <c r="F94" s="4">
         <v>42013</v>
@@ -5602,7 +5629,7 @@
       <c r="C95" s="1"/>
       <c r="D95" s="2"/>
       <c r="E95" s="3" t="s">
-        <v>439</v>
+        <v>433</v>
       </c>
       <c r="F95" s="4">
         <v>42013</v>
@@ -5618,7 +5645,7 @@
       <c r="C96" s="1"/>
       <c r="D96" s="2"/>
       <c r="E96" s="3" t="s">
-        <v>440</v>
+        <v>434</v>
       </c>
       <c r="F96" s="4">
         <v>42013</v>
@@ -5634,7 +5661,7 @@
       <c r="C97" s="1"/>
       <c r="D97" s="2"/>
       <c r="E97" s="3" t="s">
-        <v>441</v>
+        <v>435</v>
       </c>
       <c r="F97" s="4">
         <v>42013</v>
@@ -5650,7 +5677,7 @@
       <c r="C98" s="1"/>
       <c r="D98" s="2"/>
       <c r="E98" s="3" t="s">
-        <v>442</v>
+        <v>436</v>
       </c>
       <c r="F98" s="4">
         <v>42013</v>
@@ -5666,7 +5693,7 @@
       <c r="C99" s="1"/>
       <c r="D99" s="2"/>
       <c r="E99" s="3" t="s">
-        <v>443</v>
+        <v>437</v>
       </c>
       <c r="F99" s="4">
         <v>42013</v>
@@ -5682,7 +5709,7 @@
       <c r="C100" s="1"/>
       <c r="D100" s="2"/>
       <c r="E100" s="3" t="s">
-        <v>444</v>
+        <v>438</v>
       </c>
       <c r="F100" s="4">
         <v>42013</v>
@@ -5698,7 +5725,7 @@
       <c r="C101" s="1"/>
       <c r="D101" s="2"/>
       <c r="E101" s="3" t="s">
-        <v>445</v>
+        <v>439</v>
       </c>
       <c r="F101" s="4">
         <v>42013</v>
@@ -5714,7 +5741,7 @@
       <c r="C102" s="1"/>
       <c r="D102" s="2"/>
       <c r="E102" s="3" t="s">
-        <v>446</v>
+        <v>440</v>
       </c>
       <c r="F102" s="4">
         <v>42013</v>
@@ -5730,7 +5757,7 @@
       <c r="C103" s="1"/>
       <c r="D103" s="2"/>
       <c r="E103" s="3" t="s">
-        <v>447</v>
+        <v>441</v>
       </c>
       <c r="F103" s="4">
         <v>42013</v>
@@ -5746,7 +5773,7 @@
       <c r="C104" s="1"/>
       <c r="D104" s="2"/>
       <c r="E104" s="3" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
       <c r="F104" s="4">
         <v>42013</v>
@@ -5762,7 +5789,7 @@
       <c r="C105" s="1"/>
       <c r="D105" s="2"/>
       <c r="E105" s="3" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
       <c r="F105" s="4">
         <v>42013</v>
@@ -5778,7 +5805,7 @@
       <c r="C106" s="1"/>
       <c r="D106" s="2"/>
       <c r="E106" s="3" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
       <c r="F106" s="4">
         <v>42013</v>
@@ -5794,7 +5821,7 @@
       <c r="C107" s="1"/>
       <c r="D107" s="2"/>
       <c r="E107" s="3" t="s">
-        <v>451</v>
+        <v>445</v>
       </c>
       <c r="F107" s="4">
         <v>42013</v>
@@ -5810,7 +5837,7 @@
       <c r="C108" s="1"/>
       <c r="D108" s="2"/>
       <c r="E108" s="3" t="s">
-        <v>452</v>
+        <v>446</v>
       </c>
       <c r="F108" s="4">
         <v>42013</v>
@@ -5826,7 +5853,7 @@
       <c r="C109" s="1"/>
       <c r="D109" s="2"/>
       <c r="E109" s="3" t="s">
-        <v>453</v>
+        <v>447</v>
       </c>
       <c r="F109" s="4">
         <v>42013</v>
@@ -5842,7 +5869,7 @@
       <c r="C110" s="1"/>
       <c r="D110" s="2"/>
       <c r="E110" s="3" t="s">
-        <v>454</v>
+        <v>448</v>
       </c>
       <c r="F110" s="4">
         <v>42013</v>
@@ -5858,7 +5885,7 @@
       <c r="C111" s="1"/>
       <c r="D111" s="2"/>
       <c r="E111" s="3" t="s">
-        <v>455</v>
+        <v>449</v>
       </c>
       <c r="F111" s="4">
         <v>42013</v>
@@ -5874,7 +5901,7 @@
       <c r="C112" s="1"/>
       <c r="D112" s="2"/>
       <c r="E112" s="3" t="s">
-        <v>456</v>
+        <v>450</v>
       </c>
       <c r="F112" s="4">
         <v>42013</v>
@@ -5890,7 +5917,7 @@
       <c r="C113" s="1"/>
       <c r="D113" s="2"/>
       <c r="E113" s="3" t="s">
-        <v>457</v>
+        <v>451</v>
       </c>
       <c r="F113" s="4">
         <v>42013</v>
@@ -5906,7 +5933,7 @@
       <c r="C114" s="1"/>
       <c r="D114" s="2"/>
       <c r="E114" s="3" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
       <c r="F114" s="4">
         <v>42013</v>
@@ -5922,7 +5949,7 @@
       <c r="C115" s="1"/>
       <c r="D115" s="2"/>
       <c r="E115" s="3" t="s">
-        <v>459</v>
+        <v>453</v>
       </c>
       <c r="F115" s="4">
         <v>42013</v>
@@ -5938,7 +5965,7 @@
       <c r="C116" s="1"/>
       <c r="D116" s="2"/>
       <c r="E116" s="3" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="F116" s="4">
         <v>42013</v>
@@ -5954,7 +5981,7 @@
       <c r="C117" s="1"/>
       <c r="D117" s="2"/>
       <c r="E117" s="3" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="F117" s="4">
         <v>42013</v>
@@ -5970,7 +5997,7 @@
       <c r="C118" s="1"/>
       <c r="D118" s="2"/>
       <c r="E118" s="3" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
       <c r="F118" s="4">
         <v>42013</v>
@@ -5986,7 +6013,7 @@
       <c r="C119" s="1"/>
       <c r="D119" s="2"/>
       <c r="E119" s="3" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
       <c r="F119" s="4">
         <v>42013</v>
@@ -6002,7 +6029,7 @@
       <c r="C120" s="1"/>
       <c r="D120" s="2"/>
       <c r="E120" s="3" t="s">
-        <v>464</v>
+        <v>458</v>
       </c>
       <c r="F120" s="4">
         <v>42013</v>
@@ -6018,7 +6045,7 @@
       <c r="C121" s="1"/>
       <c r="D121" s="2"/>
       <c r="E121" s="3" t="s">
-        <v>465</v>
+        <v>459</v>
       </c>
       <c r="F121" s="4">
         <v>42013</v>
@@ -6034,7 +6061,7 @@
       <c r="C122" s="1"/>
       <c r="D122" s="2"/>
       <c r="E122" s="3" t="s">
-        <v>466</v>
+        <v>460</v>
       </c>
       <c r="F122" s="4">
         <v>42013</v>
@@ -6050,7 +6077,7 @@
       <c r="C123" s="1"/>
       <c r="D123" s="2"/>
       <c r="E123" s="3" t="s">
-        <v>467</v>
+        <v>461</v>
       </c>
       <c r="F123" s="4">
         <v>42013</v>
@@ -6066,7 +6093,7 @@
       <c r="C124" s="1"/>
       <c r="D124" s="2"/>
       <c r="E124" s="3" t="s">
-        <v>468</v>
+        <v>462</v>
       </c>
       <c r="F124" s="4">
         <v>42013</v>
@@ -6082,7 +6109,7 @@
       <c r="C125" s="1"/>
       <c r="D125" s="2"/>
       <c r="E125" s="3" t="s">
-        <v>469</v>
+        <v>463</v>
       </c>
       <c r="F125" s="4">
         <v>42013</v>
@@ -6098,7 +6125,7 @@
       <c r="C126" s="1"/>
       <c r="D126" s="2"/>
       <c r="E126" s="3" t="s">
-        <v>470</v>
+        <v>464</v>
       </c>
       <c r="F126" s="4">
         <v>42013</v>
@@ -6114,7 +6141,7 @@
       <c r="C127" s="1"/>
       <c r="D127" s="2"/>
       <c r="E127" s="3" t="s">
-        <v>471</v>
+        <v>465</v>
       </c>
       <c r="F127" s="4">
         <v>42013</v>
@@ -6130,7 +6157,7 @@
       <c r="C128" s="1"/>
       <c r="D128" s="2"/>
       <c r="E128" s="3" t="s">
-        <v>472</v>
+        <v>466</v>
       </c>
       <c r="F128" s="4">
         <v>42013</v>
@@ -6146,7 +6173,7 @@
       <c r="C129" s="1"/>
       <c r="D129" s="2"/>
       <c r="E129" s="3" t="s">
-        <v>473</v>
+        <v>467</v>
       </c>
       <c r="F129" s="4">
         <v>42013</v>
@@ -6162,7 +6189,7 @@
       <c r="C130" s="1"/>
       <c r="D130" s="2"/>
       <c r="E130" s="3" t="s">
-        <v>474</v>
+        <v>468</v>
       </c>
       <c r="F130" s="4">
         <v>42013</v>
@@ -6178,7 +6205,7 @@
       <c r="C131" s="1"/>
       <c r="D131" s="2"/>
       <c r="E131" s="3" t="s">
-        <v>475</v>
+        <v>469</v>
       </c>
       <c r="F131" s="4">
         <v>42013</v>
@@ -6194,7 +6221,7 @@
       <c r="C132" s="1"/>
       <c r="D132" s="2"/>
       <c r="E132" s="3" t="s">
-        <v>700</v>
+        <v>694</v>
       </c>
       <c r="F132" s="4">
         <v>42013</v>
@@ -6210,7 +6237,7 @@
       <c r="C133" s="1"/>
       <c r="D133" s="2"/>
       <c r="E133" s="3" t="s">
-        <v>701</v>
+        <v>695</v>
       </c>
       <c r="F133" s="4">
         <v>42013</v>
@@ -6226,7 +6253,7 @@
       <c r="C134" s="1"/>
       <c r="D134" s="2"/>
       <c r="E134" s="3" t="s">
-        <v>476</v>
+        <v>470</v>
       </c>
       <c r="F134" s="4">
         <v>42013</v>
@@ -6242,7 +6269,7 @@
       <c r="C135" s="1"/>
       <c r="D135" s="2"/>
       <c r="E135" s="3" t="s">
-        <v>477</v>
+        <v>471</v>
       </c>
       <c r="F135" s="4">
         <v>42013</v>
@@ -6258,7 +6285,7 @@
       <c r="C136" s="1"/>
       <c r="D136" s="2"/>
       <c r="E136" s="3" t="s">
-        <v>478</v>
+        <v>472</v>
       </c>
       <c r="F136" s="4">
         <v>42013</v>
@@ -6274,7 +6301,7 @@
       <c r="C137" s="1"/>
       <c r="D137" s="2"/>
       <c r="E137" s="3" t="s">
-        <v>479</v>
+        <v>473</v>
       </c>
       <c r="F137" s="4">
         <v>42013</v>
@@ -6290,7 +6317,7 @@
       <c r="C138" s="1"/>
       <c r="D138" s="2"/>
       <c r="E138" s="3" t="s">
-        <v>480</v>
+        <v>474</v>
       </c>
       <c r="F138" s="4">
         <v>42013</v>
@@ -6306,7 +6333,7 @@
       <c r="C139" s="1"/>
       <c r="D139" s="2"/>
       <c r="E139" s="3" t="s">
-        <v>481</v>
+        <v>475</v>
       </c>
       <c r="F139" s="4">
         <v>42013</v>
@@ -6322,7 +6349,7 @@
       <c r="C140" s="1"/>
       <c r="D140" s="2"/>
       <c r="E140" s="3" t="s">
-        <v>482</v>
+        <v>476</v>
       </c>
       <c r="F140" s="4">
         <v>42013</v>
@@ -6338,7 +6365,7 @@
       <c r="C141" s="1"/>
       <c r="D141" s="2"/>
       <c r="E141" s="3" t="s">
-        <v>483</v>
+        <v>477</v>
       </c>
       <c r="F141" s="4">
         <v>42013</v>
@@ -6354,7 +6381,7 @@
       <c r="C142" s="1"/>
       <c r="D142" s="2"/>
       <c r="E142" s="3" t="s">
-        <v>484</v>
+        <v>478</v>
       </c>
       <c r="F142" s="4">
         <v>42013</v>
@@ -6370,7 +6397,7 @@
       <c r="C143" s="1"/>
       <c r="D143" s="2"/>
       <c r="E143" s="3" t="s">
-        <v>485</v>
+        <v>479</v>
       </c>
       <c r="F143" s="4">
         <v>42013</v>
@@ -6386,7 +6413,7 @@
       <c r="C144" s="1"/>
       <c r="D144" s="2"/>
       <c r="E144" s="3" t="s">
-        <v>486</v>
+        <v>480</v>
       </c>
       <c r="F144" s="4">
         <v>42013</v>
@@ -6402,7 +6429,7 @@
       <c r="C145" s="1"/>
       <c r="D145" s="2"/>
       <c r="E145" s="3" t="s">
-        <v>487</v>
+        <v>481</v>
       </c>
       <c r="F145" s="4">
         <v>42013</v>
@@ -6418,7 +6445,7 @@
       <c r="C146" s="1"/>
       <c r="D146" s="2"/>
       <c r="E146" s="3" t="s">
-        <v>488</v>
+        <v>482</v>
       </c>
       <c r="F146" s="4">
         <v>42013</v>
@@ -6434,7 +6461,7 @@
       <c r="C147" s="1"/>
       <c r="D147" s="2"/>
       <c r="E147" s="3" t="s">
-        <v>489</v>
+        <v>483</v>
       </c>
       <c r="F147" s="4">
         <v>42013</v>
@@ -6450,7 +6477,7 @@
       <c r="C148" s="1"/>
       <c r="D148" s="2"/>
       <c r="E148" s="3" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="F148" s="4">
         <v>42013</v>
@@ -6466,7 +6493,7 @@
       <c r="C149" s="1"/>
       <c r="D149" s="2"/>
       <c r="E149" s="3" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="F149" s="4">
         <v>42013</v>
@@ -6482,7 +6509,7 @@
       <c r="C150" s="1"/>
       <c r="D150" s="2"/>
       <c r="E150" s="3" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="F150" s="4">
         <v>42013</v>
@@ -6498,7 +6525,7 @@
       <c r="C151" s="1"/>
       <c r="D151" s="2"/>
       <c r="E151" s="3" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="F151" s="4">
         <v>42013</v>
@@ -6514,7 +6541,7 @@
       <c r="C152" s="1"/>
       <c r="D152" s="2"/>
       <c r="E152" s="3" t="s">
-        <v>491</v>
+        <v>485</v>
       </c>
       <c r="F152" s="4">
         <v>42013</v>
@@ -6530,7 +6557,7 @@
       <c r="C153" s="1"/>
       <c r="D153" s="2"/>
       <c r="E153" s="3" t="s">
-        <v>492</v>
+        <v>486</v>
       </c>
       <c r="F153" s="4">
         <v>42013</v>
@@ -6546,7 +6573,7 @@
       <c r="C154" s="1"/>
       <c r="D154" s="2"/>
       <c r="E154" s="3" t="s">
-        <v>493</v>
+        <v>487</v>
       </c>
       <c r="F154" s="4">
         <v>42013</v>
@@ -6562,7 +6589,7 @@
       <c r="C155" s="1"/>
       <c r="D155" s="2"/>
       <c r="E155" s="3" t="s">
-        <v>494</v>
+        <v>488</v>
       </c>
       <c r="F155" s="4">
         <v>42013</v>
@@ -6578,7 +6605,7 @@
       <c r="C156" s="1"/>
       <c r="D156" s="2"/>
       <c r="E156" s="3" t="s">
-        <v>495</v>
+        <v>489</v>
       </c>
       <c r="F156" s="4">
         <v>42013</v>
@@ -6594,7 +6621,7 @@
       <c r="C157" s="1"/>
       <c r="D157" s="2"/>
       <c r="E157" s="3" t="s">
-        <v>496</v>
+        <v>490</v>
       </c>
       <c r="F157" s="4">
         <v>42013</v>
@@ -6610,7 +6637,7 @@
       <c r="C158" s="1"/>
       <c r="D158" s="2"/>
       <c r="E158" s="3" t="s">
-        <v>497</v>
+        <v>491</v>
       </c>
       <c r="F158" s="4">
         <v>42013</v>
@@ -6626,7 +6653,7 @@
       <c r="C159" s="1"/>
       <c r="D159" s="2"/>
       <c r="E159" s="3" t="s">
-        <v>498</v>
+        <v>492</v>
       </c>
       <c r="F159" s="4">
         <v>42013</v>
@@ -6642,7 +6669,7 @@
       <c r="C160" s="1"/>
       <c r="D160" s="2"/>
       <c r="E160" s="3" t="s">
-        <v>499</v>
+        <v>493</v>
       </c>
       <c r="F160" s="4">
         <v>42013</v>
@@ -6658,7 +6685,7 @@
       <c r="C161" s="1"/>
       <c r="D161" s="2"/>
       <c r="E161" s="3" t="s">
-        <v>500</v>
+        <v>494</v>
       </c>
       <c r="F161" s="4">
         <v>42013</v>
@@ -6674,7 +6701,7 @@
       <c r="C162" s="1"/>
       <c r="D162" s="2"/>
       <c r="E162" s="3" t="s">
-        <v>501</v>
+        <v>495</v>
       </c>
       <c r="F162" s="4">
         <v>42013</v>
@@ -6690,7 +6717,7 @@
       <c r="C163" s="1"/>
       <c r="D163" s="2"/>
       <c r="E163" s="3" t="s">
-        <v>502</v>
+        <v>496</v>
       </c>
       <c r="F163" s="4">
         <v>42013</v>
@@ -6706,7 +6733,7 @@
       <c r="C164" s="1"/>
       <c r="D164" s="2"/>
       <c r="E164" s="3" t="s">
-        <v>503</v>
+        <v>497</v>
       </c>
       <c r="F164" s="4">
         <v>42013</v>
@@ -6722,7 +6749,7 @@
       <c r="C165" s="1"/>
       <c r="D165" s="2"/>
       <c r="E165" s="3" t="s">
-        <v>504</v>
+        <v>498</v>
       </c>
       <c r="F165" s="4">
         <v>42013</v>
@@ -6738,7 +6765,7 @@
       <c r="C166" s="1"/>
       <c r="D166" s="2"/>
       <c r="E166" s="3" t="s">
-        <v>505</v>
+        <v>499</v>
       </c>
       <c r="F166" s="4">
         <v>42013</v>
@@ -6754,7 +6781,7 @@
       <c r="C167" s="1"/>
       <c r="D167" s="2"/>
       <c r="E167" s="3" t="s">
-        <v>506</v>
+        <v>500</v>
       </c>
       <c r="F167" s="4">
         <v>42013</v>
@@ -6770,7 +6797,7 @@
       <c r="C168" s="1"/>
       <c r="D168" s="2"/>
       <c r="E168" s="3" t="s">
-        <v>507</v>
+        <v>501</v>
       </c>
       <c r="F168" s="4">
         <v>42013</v>
@@ -6786,7 +6813,7 @@
       <c r="C169" s="1"/>
       <c r="D169" s="2"/>
       <c r="E169" s="3" t="s">
-        <v>508</v>
+        <v>502</v>
       </c>
       <c r="F169" s="4">
         <v>42013</v>
@@ -6802,7 +6829,7 @@
       <c r="C170" s="1"/>
       <c r="D170" s="2"/>
       <c r="E170" s="3" t="s">
-        <v>509</v>
+        <v>503</v>
       </c>
       <c r="F170" s="4">
         <v>42013</v>
@@ -6818,7 +6845,7 @@
       <c r="C171" s="1"/>
       <c r="D171" s="2"/>
       <c r="E171" s="3" t="s">
-        <v>510</v>
+        <v>504</v>
       </c>
       <c r="F171" s="4">
         <v>42013</v>
@@ -6834,7 +6861,7 @@
       <c r="C172" s="1"/>
       <c r="D172" s="2"/>
       <c r="E172" s="3" t="s">
-        <v>511</v>
+        <v>505</v>
       </c>
       <c r="F172" s="4">
         <v>42013</v>
@@ -6850,7 +6877,7 @@
       <c r="C173" s="1"/>
       <c r="D173" s="2"/>
       <c r="E173" s="3" t="s">
-        <v>512</v>
+        <v>506</v>
       </c>
       <c r="F173" s="4">
         <v>42013</v>
@@ -6866,7 +6893,7 @@
       <c r="C174" s="1"/>
       <c r="D174" s="2"/>
       <c r="E174" s="3" t="s">
-        <v>513</v>
+        <v>507</v>
       </c>
       <c r="F174" s="4">
         <v>42013</v>
@@ -6882,7 +6909,7 @@
       <c r="C175" s="1"/>
       <c r="D175" s="2"/>
       <c r="E175" s="3" t="s">
-        <v>514</v>
+        <v>508</v>
       </c>
       <c r="F175" s="4">
         <v>42013</v>
@@ -6898,7 +6925,7 @@
       <c r="C176" s="1"/>
       <c r="D176" s="2"/>
       <c r="E176" s="3" t="s">
-        <v>515</v>
+        <v>509</v>
       </c>
       <c r="F176" s="4">
         <v>42013</v>
@@ -6914,7 +6941,7 @@
       <c r="C177" s="1"/>
       <c r="D177" s="2"/>
       <c r="E177" s="3" t="s">
-        <v>516</v>
+        <v>510</v>
       </c>
       <c r="F177" s="4">
         <v>42013</v>
@@ -6930,7 +6957,7 @@
       <c r="C178" s="1"/>
       <c r="D178" s="2"/>
       <c r="E178" s="3" t="s">
-        <v>517</v>
+        <v>511</v>
       </c>
       <c r="F178" s="4">
         <v>42013</v>
@@ -6946,7 +6973,7 @@
       <c r="C179" s="1"/>
       <c r="D179" s="2"/>
       <c r="E179" s="3" t="s">
-        <v>518</v>
+        <v>512</v>
       </c>
       <c r="F179" s="4">
         <v>42013</v>
@@ -6962,7 +6989,7 @@
       <c r="C180" s="1"/>
       <c r="D180" s="2"/>
       <c r="E180" s="3" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
       <c r="F180" s="4">
         <v>42013</v>
@@ -6978,7 +7005,7 @@
       <c r="C181" s="1"/>
       <c r="D181" s="2"/>
       <c r="E181" s="3" t="s">
-        <v>520</v>
+        <v>514</v>
       </c>
       <c r="F181" s="4">
         <v>42013</v>
@@ -6994,7 +7021,7 @@
       <c r="C182" s="1"/>
       <c r="D182" s="2"/>
       <c r="E182" s="3" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="F182" s="4">
         <v>42013</v>
@@ -7010,7 +7037,7 @@
       <c r="C183" s="1"/>
       <c r="D183" s="2"/>
       <c r="E183" s="3" t="s">
-        <v>522</v>
+        <v>516</v>
       </c>
       <c r="F183" s="4">
         <v>42013</v>
@@ -7026,7 +7053,7 @@
       <c r="C184" s="1"/>
       <c r="D184" s="2"/>
       <c r="E184" s="3" t="s">
-        <v>523</v>
+        <v>517</v>
       </c>
       <c r="F184" s="4">
         <v>42013</v>
@@ -7042,7 +7069,7 @@
       <c r="C185" s="1"/>
       <c r="D185" s="2"/>
       <c r="E185" s="3" t="s">
-        <v>524</v>
+        <v>518</v>
       </c>
       <c r="F185" s="4">
         <v>42013</v>
@@ -7058,7 +7085,7 @@
       <c r="C186" s="1"/>
       <c r="D186" s="2"/>
       <c r="E186" s="3" t="s">
-        <v>525</v>
+        <v>519</v>
       </c>
       <c r="F186" s="4">
         <v>42013</v>
@@ -7074,7 +7101,7 @@
       <c r="C187" s="1"/>
       <c r="D187" s="2"/>
       <c r="E187" s="3" t="s">
-        <v>526</v>
+        <v>520</v>
       </c>
       <c r="F187" s="4">
         <v>42013</v>
@@ -7090,7 +7117,7 @@
       <c r="C188" s="1"/>
       <c r="D188" s="2"/>
       <c r="E188" s="3" t="s">
-        <v>527</v>
+        <v>521</v>
       </c>
       <c r="F188" s="4">
         <v>42013</v>
@@ -7106,7 +7133,7 @@
       <c r="C189" s="1"/>
       <c r="D189" s="2"/>
       <c r="E189" s="3" t="s">
-        <v>528</v>
+        <v>522</v>
       </c>
       <c r="F189" s="4">
         <v>42013</v>
@@ -7122,7 +7149,7 @@
       <c r="C190" s="1"/>
       <c r="D190" s="2"/>
       <c r="E190" s="3" t="s">
-        <v>529</v>
+        <v>523</v>
       </c>
       <c r="F190" s="4">
         <v>42013</v>
@@ -7138,7 +7165,7 @@
       <c r="C191" s="1"/>
       <c r="D191" s="2"/>
       <c r="E191" s="3" t="s">
-        <v>530</v>
+        <v>524</v>
       </c>
       <c r="F191" s="4">
         <v>42013</v>
@@ -7154,7 +7181,7 @@
       <c r="C192" s="1"/>
       <c r="D192" s="2"/>
       <c r="E192" s="3" t="s">
-        <v>531</v>
+        <v>525</v>
       </c>
       <c r="F192" s="4">
         <v>42013</v>
@@ -7170,7 +7197,7 @@
       <c r="C193" s="1"/>
       <c r="D193" s="2"/>
       <c r="E193" s="3" t="s">
-        <v>532</v>
+        <v>526</v>
       </c>
       <c r="F193" s="4">
         <v>42013</v>
@@ -7186,7 +7213,7 @@
       <c r="C194" s="1"/>
       <c r="D194" s="2"/>
       <c r="E194" s="3" t="s">
-        <v>533</v>
+        <v>527</v>
       </c>
       <c r="F194" s="4">
         <v>42013</v>
@@ -7202,7 +7229,7 @@
       <c r="C195" s="1"/>
       <c r="D195" s="2"/>
       <c r="E195" s="3" t="s">
-        <v>534</v>
+        <v>528</v>
       </c>
       <c r="F195" s="4">
         <v>42013</v>
@@ -7218,7 +7245,7 @@
       <c r="C196" s="1"/>
       <c r="D196" s="2"/>
       <c r="E196" s="3" t="s">
-        <v>535</v>
+        <v>529</v>
       </c>
       <c r="F196" s="4">
         <v>42013</v>
@@ -7234,7 +7261,7 @@
       <c r="C197" s="1"/>
       <c r="D197" s="2"/>
       <c r="E197" s="3" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
       <c r="F197" s="4">
         <v>42013</v>
@@ -7250,7 +7277,7 @@
       <c r="C198" s="1"/>
       <c r="D198" s="2"/>
       <c r="E198" s="3" t="s">
-        <v>537</v>
+        <v>531</v>
       </c>
       <c r="F198" s="4">
         <v>42013</v>
@@ -7266,7 +7293,7 @@
       <c r="C199" s="1"/>
       <c r="D199" s="2"/>
       <c r="E199" s="3" t="s">
-        <v>538</v>
+        <v>532</v>
       </c>
       <c r="F199" s="4">
         <v>42013</v>
@@ -7282,7 +7309,7 @@
       <c r="C200" s="1"/>
       <c r="D200" s="2"/>
       <c r="E200" s="3" t="s">
-        <v>539</v>
+        <v>533</v>
       </c>
       <c r="F200" s="4">
         <v>42013</v>
@@ -7298,7 +7325,7 @@
       <c r="C201" s="1"/>
       <c r="D201" s="2"/>
       <c r="E201" s="3" t="s">
-        <v>540</v>
+        <v>534</v>
       </c>
       <c r="F201" s="4">
         <v>42013</v>
@@ -7314,7 +7341,7 @@
       <c r="C202" s="1"/>
       <c r="D202" s="2"/>
       <c r="E202" s="3" t="s">
-        <v>541</v>
+        <v>535</v>
       </c>
       <c r="F202" s="4">
         <v>42013</v>
@@ -7330,7 +7357,7 @@
       <c r="C203" s="1"/>
       <c r="D203" s="2"/>
       <c r="E203" s="3" t="s">
-        <v>542</v>
+        <v>536</v>
       </c>
       <c r="F203" s="4">
         <v>42013</v>
@@ -7346,7 +7373,7 @@
       <c r="C204" s="1"/>
       <c r="D204" s="2"/>
       <c r="E204" s="3" t="s">
-        <v>543</v>
+        <v>537</v>
       </c>
       <c r="F204" s="4">
         <v>42013</v>
@@ -7362,7 +7389,7 @@
       <c r="C205" s="1"/>
       <c r="D205" s="2"/>
       <c r="E205" s="3" t="s">
-        <v>544</v>
+        <v>538</v>
       </c>
       <c r="F205" s="4">
         <v>42013</v>
@@ -7378,7 +7405,7 @@
       <c r="C206" s="1"/>
       <c r="D206" s="2"/>
       <c r="E206" s="3" t="s">
-        <v>545</v>
+        <v>539</v>
       </c>
       <c r="F206" s="4">
         <v>42013</v>
@@ -7394,7 +7421,7 @@
       <c r="C207" s="1"/>
       <c r="D207" s="2"/>
       <c r="E207" s="3" t="s">
-        <v>546</v>
+        <v>540</v>
       </c>
       <c r="F207" s="4">
         <v>42013</v>
@@ -7410,7 +7437,7 @@
       <c r="C208" s="1"/>
       <c r="D208" s="2"/>
       <c r="E208" s="3" t="s">
-        <v>547</v>
+        <v>541</v>
       </c>
       <c r="F208" s="4">
         <v>42013</v>
@@ -7426,7 +7453,7 @@
       <c r="C209" s="1"/>
       <c r="D209" s="2"/>
       <c r="E209" s="3" t="s">
-        <v>548</v>
+        <v>542</v>
       </c>
       <c r="F209" s="4">
         <v>42013</v>
@@ -7442,7 +7469,7 @@
       <c r="C210" s="1"/>
       <c r="D210" s="2"/>
       <c r="E210" s="3" t="s">
-        <v>549</v>
+        <v>543</v>
       </c>
       <c r="F210" s="4">
         <v>42013</v>
@@ -7458,7 +7485,7 @@
       <c r="C211" s="1"/>
       <c r="D211" s="2"/>
       <c r="E211" s="3" t="s">
-        <v>550</v>
+        <v>544</v>
       </c>
       <c r="F211" s="4">
         <v>42013</v>
@@ -7474,7 +7501,7 @@
       <c r="C212" s="1"/>
       <c r="D212" s="2"/>
       <c r="E212" s="3" t="s">
-        <v>551</v>
+        <v>545</v>
       </c>
       <c r="F212" s="4">
         <v>42013</v>
@@ -7490,7 +7517,7 @@
       <c r="C213" s="1"/>
       <c r="D213" s="2"/>
       <c r="E213" s="3" t="s">
-        <v>552</v>
+        <v>546</v>
       </c>
       <c r="F213" s="4">
         <v>42013</v>
@@ -7506,7 +7533,7 @@
       <c r="C214" s="1"/>
       <c r="D214" s="2"/>
       <c r="E214" s="3" t="s">
-        <v>553</v>
+        <v>547</v>
       </c>
       <c r="F214" s="4">
         <v>42013</v>
@@ -7522,7 +7549,7 @@
       <c r="C215" s="1"/>
       <c r="D215" s="2"/>
       <c r="E215" s="3" t="s">
-        <v>554</v>
+        <v>548</v>
       </c>
       <c r="F215" s="4">
         <v>42013</v>
@@ -7538,7 +7565,7 @@
       <c r="C216" s="1"/>
       <c r="D216" s="2"/>
       <c r="E216" s="3" t="s">
-        <v>555</v>
+        <v>549</v>
       </c>
       <c r="F216" s="4">
         <v>42013</v>
@@ -7554,7 +7581,7 @@
       <c r="C217" s="1"/>
       <c r="D217" s="2"/>
       <c r="E217" s="3" t="s">
-        <v>556</v>
+        <v>550</v>
       </c>
       <c r="F217" s="4">
         <v>42013</v>
@@ -7570,7 +7597,7 @@
       <c r="C218" s="1"/>
       <c r="D218" s="2"/>
       <c r="E218" s="3" t="s">
-        <v>557</v>
+        <v>551</v>
       </c>
       <c r="F218" s="4">
         <v>42013</v>
@@ -7586,7 +7613,7 @@
       <c r="C219" s="1"/>
       <c r="D219" s="2"/>
       <c r="E219" s="3" t="s">
-        <v>558</v>
+        <v>552</v>
       </c>
       <c r="F219" s="4">
         <v>42013</v>
@@ -7602,7 +7629,7 @@
       <c r="C220" s="1"/>
       <c r="D220" s="2"/>
       <c r="E220" s="3" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
       <c r="F220" s="4">
         <v>42013</v>
@@ -7618,7 +7645,7 @@
       <c r="C221" s="1"/>
       <c r="D221" s="2"/>
       <c r="E221" s="3" t="s">
-        <v>560</v>
+        <v>554</v>
       </c>
       <c r="F221" s="4">
         <v>42013</v>
@@ -7634,7 +7661,7 @@
       <c r="C222" s="1"/>
       <c r="D222" s="2"/>
       <c r="E222" s="3" t="s">
-        <v>561</v>
+        <v>555</v>
       </c>
       <c r="F222" s="4">
         <v>42013</v>
@@ -7650,7 +7677,7 @@
       <c r="C223" s="1"/>
       <c r="D223" s="2"/>
       <c r="E223" s="3" t="s">
-        <v>562</v>
+        <v>556</v>
       </c>
       <c r="F223" s="4">
         <v>42013</v>
@@ -7666,7 +7693,7 @@
       <c r="C224" s="1"/>
       <c r="D224" s="2"/>
       <c r="E224" s="3" t="s">
-        <v>563</v>
+        <v>557</v>
       </c>
       <c r="F224" s="4">
         <v>42013</v>
@@ -7682,7 +7709,7 @@
       <c r="C225" s="1"/>
       <c r="D225" s="2"/>
       <c r="E225" s="3" t="s">
-        <v>564</v>
+        <v>558</v>
       </c>
       <c r="F225" s="4">
         <v>42013</v>
@@ -7698,7 +7725,7 @@
       <c r="C226" s="1"/>
       <c r="D226" s="2"/>
       <c r="E226" s="3" t="s">
-        <v>565</v>
+        <v>559</v>
       </c>
       <c r="F226" s="4">
         <v>42013</v>
@@ -7714,7 +7741,7 @@
       <c r="C227" s="1"/>
       <c r="D227" s="2"/>
       <c r="E227" s="3" t="s">
-        <v>566</v>
+        <v>560</v>
       </c>
       <c r="F227" s="4">
         <v>42013</v>
@@ -7730,7 +7757,7 @@
       <c r="C228" s="1"/>
       <c r="D228" s="2"/>
       <c r="E228" s="3" t="s">
-        <v>567</v>
+        <v>561</v>
       </c>
       <c r="F228" s="4">
         <v>42013</v>
@@ -7746,7 +7773,7 @@
       <c r="C229" s="1"/>
       <c r="D229" s="2"/>
       <c r="E229" s="3" t="s">
-        <v>568</v>
+        <v>562</v>
       </c>
       <c r="F229" s="4">
         <v>42013</v>
@@ -7762,7 +7789,7 @@
       <c r="C230" s="1"/>
       <c r="D230" s="2"/>
       <c r="E230" s="3" t="s">
-        <v>569</v>
+        <v>563</v>
       </c>
       <c r="F230" s="4">
         <v>42013</v>
@@ -7778,7 +7805,7 @@
       <c r="C231" s="1"/>
       <c r="D231" s="2"/>
       <c r="E231" s="3" t="s">
-        <v>570</v>
+        <v>564</v>
       </c>
       <c r="F231" s="4">
         <v>42013</v>
@@ -7794,7 +7821,7 @@
       <c r="C232" s="1"/>
       <c r="D232" s="2"/>
       <c r="E232" s="3" t="s">
-        <v>571</v>
+        <v>565</v>
       </c>
       <c r="F232" s="4">
         <v>42013</v>
@@ -7810,7 +7837,7 @@
       <c r="C233" s="1"/>
       <c r="D233" s="2"/>
       <c r="E233" s="3" t="s">
-        <v>572</v>
+        <v>566</v>
       </c>
       <c r="F233" s="4">
         <v>42013</v>
@@ -7826,7 +7853,7 @@
       <c r="C234" s="1"/>
       <c r="D234" s="2"/>
       <c r="E234" s="3" t="s">
-        <v>573</v>
+        <v>567</v>
       </c>
       <c r="F234" s="4">
         <v>42013</v>
@@ -7842,7 +7869,7 @@
       <c r="C235" s="1"/>
       <c r="D235" s="2"/>
       <c r="E235" s="3" t="s">
-        <v>574</v>
+        <v>568</v>
       </c>
       <c r="F235" s="4">
         <v>42013</v>
@@ -7858,7 +7885,7 @@
       <c r="C236" s="1"/>
       <c r="D236" s="2"/>
       <c r="E236" s="3" t="s">
-        <v>575</v>
+        <v>569</v>
       </c>
       <c r="F236" s="4">
         <v>42013</v>
@@ -7874,7 +7901,7 @@
       <c r="C237" s="1"/>
       <c r="D237" s="2"/>
       <c r="E237" s="3" t="s">
-        <v>576</v>
+        <v>570</v>
       </c>
       <c r="F237" s="4">
         <v>42013</v>
@@ -7890,7 +7917,7 @@
       <c r="C238" s="1"/>
       <c r="D238" s="2"/>
       <c r="E238" s="3" t="s">
-        <v>577</v>
+        <v>571</v>
       </c>
       <c r="F238" s="4">
         <v>42013</v>
@@ -7906,7 +7933,7 @@
       <c r="C239" s="1"/>
       <c r="D239" s="2"/>
       <c r="E239" s="3" t="s">
-        <v>578</v>
+        <v>572</v>
       </c>
       <c r="F239" s="4">
         <v>42013</v>
@@ -7922,7 +7949,7 @@
       <c r="C240" s="1"/>
       <c r="D240" s="2"/>
       <c r="E240" s="3" t="s">
-        <v>579</v>
+        <v>573</v>
       </c>
       <c r="F240" s="4">
         <v>42013</v>
@@ -7938,7 +7965,7 @@
       <c r="C241" s="1"/>
       <c r="D241" s="2"/>
       <c r="E241" s="3" t="s">
-        <v>580</v>
+        <v>574</v>
       </c>
       <c r="F241" s="4">
         <v>42013</v>
@@ -7954,7 +7981,7 @@
       <c r="C242" s="1"/>
       <c r="D242" s="2"/>
       <c r="E242" s="3" t="s">
-        <v>581</v>
+        <v>575</v>
       </c>
       <c r="F242" s="4">
         <v>42013</v>
@@ -7970,7 +7997,7 @@
       <c r="C243" s="1"/>
       <c r="D243" s="2"/>
       <c r="E243" s="3" t="s">
-        <v>582</v>
+        <v>576</v>
       </c>
       <c r="F243" s="4">
         <v>42013</v>
@@ -7986,7 +8013,7 @@
       <c r="C244" s="1"/>
       <c r="D244" s="2"/>
       <c r="E244" s="3" t="s">
-        <v>583</v>
+        <v>577</v>
       </c>
       <c r="F244" s="4">
         <v>42013</v>
@@ -8002,7 +8029,7 @@
       <c r="C245" s="1"/>
       <c r="D245" s="2"/>
       <c r="E245" s="3" t="s">
-        <v>584</v>
+        <v>578</v>
       </c>
       <c r="F245" s="4">
         <v>42013</v>
@@ -8018,7 +8045,7 @@
       <c r="C246" s="1"/>
       <c r="D246" s="2"/>
       <c r="E246" s="3" t="s">
-        <v>585</v>
+        <v>579</v>
       </c>
       <c r="F246" s="4">
         <v>42013</v>
@@ -8034,7 +8061,7 @@
       <c r="C247" s="1"/>
       <c r="D247" s="2"/>
       <c r="E247" s="3" t="s">
-        <v>586</v>
+        <v>580</v>
       </c>
       <c r="F247" s="4">
         <v>42013</v>
@@ -8050,7 +8077,7 @@
       <c r="C248" s="1"/>
       <c r="D248" s="2"/>
       <c r="E248" s="3" t="s">
-        <v>587</v>
+        <v>581</v>
       </c>
       <c r="F248" s="4">
         <v>42013</v>
@@ -8066,7 +8093,7 @@
       <c r="C249" s="1"/>
       <c r="D249" s="2"/>
       <c r="E249" s="3" t="s">
-        <v>588</v>
+        <v>582</v>
       </c>
       <c r="F249" s="4">
         <v>42013</v>
@@ -8082,7 +8109,7 @@
       <c r="C250" s="1"/>
       <c r="D250" s="2"/>
       <c r="E250" s="3" t="s">
-        <v>589</v>
+        <v>583</v>
       </c>
       <c r="F250" s="4">
         <v>42013</v>
@@ -8098,7 +8125,7 @@
       <c r="C251" s="1"/>
       <c r="D251" s="2"/>
       <c r="E251" s="3" t="s">
-        <v>590</v>
+        <v>584</v>
       </c>
       <c r="F251" s="4">
         <v>42013</v>
@@ -8114,7 +8141,7 @@
       <c r="C252" s="1"/>
       <c r="D252" s="2"/>
       <c r="E252" s="3" t="s">
-        <v>591</v>
+        <v>585</v>
       </c>
       <c r="F252" s="4">
         <v>42013</v>
@@ -8130,7 +8157,7 @@
       <c r="C253" s="1"/>
       <c r="D253" s="2"/>
       <c r="E253" s="3" t="s">
-        <v>592</v>
+        <v>586</v>
       </c>
       <c r="F253" s="4">
         <v>42013</v>
@@ -8146,7 +8173,7 @@
       <c r="C254" s="1"/>
       <c r="D254" s="2"/>
       <c r="E254" s="3" t="s">
-        <v>593</v>
+        <v>587</v>
       </c>
       <c r="F254" s="4">
         <v>42013</v>
@@ -8162,7 +8189,7 @@
       <c r="C255" s="1"/>
       <c r="D255" s="2"/>
       <c r="E255" s="3" t="s">
-        <v>594</v>
+        <v>588</v>
       </c>
       <c r="F255" s="4">
         <v>42013</v>
@@ -8178,7 +8205,7 @@
       <c r="C256" s="1"/>
       <c r="D256" s="2"/>
       <c r="E256" s="3" t="s">
-        <v>595</v>
+        <v>589</v>
       </c>
       <c r="F256" s="4">
         <v>42013</v>
@@ -8194,7 +8221,7 @@
       <c r="C257" s="1"/>
       <c r="D257" s="2"/>
       <c r="E257" s="3" t="s">
-        <v>596</v>
+        <v>590</v>
       </c>
       <c r="F257" s="4">
         <v>42013</v>
@@ -8210,7 +8237,7 @@
       <c r="C258" s="1"/>
       <c r="D258" s="2"/>
       <c r="E258" s="3" t="s">
-        <v>597</v>
+        <v>591</v>
       </c>
       <c r="F258" s="4">
         <v>42013</v>
@@ -8226,7 +8253,7 @@
       <c r="C259" s="1"/>
       <c r="D259" s="2"/>
       <c r="E259" s="3" t="s">
-        <v>598</v>
+        <v>592</v>
       </c>
       <c r="F259" s="4">
         <v>42013</v>
@@ -8242,7 +8269,7 @@
       <c r="C260" s="1"/>
       <c r="D260" s="2"/>
       <c r="E260" s="3" t="s">
-        <v>599</v>
+        <v>593</v>
       </c>
       <c r="F260" s="4">
         <v>42013</v>
@@ -8258,7 +8285,7 @@
       <c r="C261" s="1"/>
       <c r="D261" s="2"/>
       <c r="E261" s="3" t="s">
-        <v>600</v>
+        <v>594</v>
       </c>
       <c r="F261" s="4">
         <v>42013</v>
@@ -8274,7 +8301,7 @@
       <c r="C262" s="1"/>
       <c r="D262" s="2"/>
       <c r="E262" s="3" t="s">
-        <v>601</v>
+        <v>595</v>
       </c>
       <c r="F262" s="4">
         <v>42013</v>
@@ -8290,7 +8317,7 @@
       <c r="C263" s="1"/>
       <c r="D263" s="2"/>
       <c r="E263" s="3" t="s">
-        <v>602</v>
+        <v>596</v>
       </c>
       <c r="F263" s="4">
         <v>42013</v>
@@ -8306,7 +8333,7 @@
       <c r="C264" s="1"/>
       <c r="D264" s="2"/>
       <c r="E264" s="3" t="s">
-        <v>603</v>
+        <v>597</v>
       </c>
       <c r="F264" s="4">
         <v>42013</v>
@@ -8322,7 +8349,7 @@
       <c r="C265" s="1"/>
       <c r="D265" s="2"/>
       <c r="E265" s="3" t="s">
-        <v>604</v>
+        <v>598</v>
       </c>
       <c r="F265" s="4">
         <v>42013</v>
@@ -8338,7 +8365,7 @@
       <c r="C266" s="1"/>
       <c r="D266" s="2"/>
       <c r="E266" s="3" t="s">
-        <v>605</v>
+        <v>599</v>
       </c>
       <c r="F266" s="4">
         <v>42013</v>
@@ -8354,7 +8381,7 @@
       <c r="C267" s="1"/>
       <c r="D267" s="2"/>
       <c r="E267" s="3" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="F267" s="4">
         <v>42013</v>
@@ -8370,7 +8397,7 @@
       <c r="C268" s="1"/>
       <c r="D268" s="2"/>
       <c r="E268" s="3" t="s">
-        <v>607</v>
+        <v>601</v>
       </c>
       <c r="F268" s="4">
         <v>42013</v>
@@ -8386,7 +8413,7 @@
       <c r="C269" s="1"/>
       <c r="D269" s="2"/>
       <c r="E269" s="3" t="s">
-        <v>608</v>
+        <v>602</v>
       </c>
       <c r="F269" s="4">
         <v>42013</v>
@@ -8402,7 +8429,7 @@
       <c r="C270" s="1"/>
       <c r="D270" s="2"/>
       <c r="E270" s="3" t="s">
-        <v>609</v>
+        <v>603</v>
       </c>
       <c r="F270" s="4">
         <v>42013</v>
@@ -8418,7 +8445,7 @@
       <c r="C271" s="1"/>
       <c r="D271" s="2"/>
       <c r="E271" s="3" t="s">
-        <v>610</v>
+        <v>604</v>
       </c>
       <c r="F271" s="4">
         <v>42013</v>
@@ -8434,7 +8461,7 @@
       <c r="C272" s="1"/>
       <c r="D272" s="2"/>
       <c r="E272" s="3" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="F272" s="4">
         <v>42013</v>
@@ -8450,7 +8477,7 @@
       <c r="C273" s="1"/>
       <c r="D273" s="2"/>
       <c r="E273" s="3" t="s">
-        <v>612</v>
+        <v>606</v>
       </c>
       <c r="F273" s="4">
         <v>42013</v>
@@ -8466,7 +8493,7 @@
       <c r="C274" s="1"/>
       <c r="D274" s="2"/>
       <c r="E274" s="3" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="F274" s="4">
         <v>42013</v>
@@ -8482,7 +8509,7 @@
       <c r="C275" s="1"/>
       <c r="D275" s="2"/>
       <c r="E275" s="3" t="s">
-        <v>614</v>
+        <v>608</v>
       </c>
       <c r="F275" s="4">
         <v>42013</v>
@@ -8498,7 +8525,7 @@
       <c r="C276" s="1"/>
       <c r="D276" s="2"/>
       <c r="E276" s="3" t="s">
-        <v>615</v>
+        <v>609</v>
       </c>
       <c r="F276" s="4">
         <v>42013</v>
@@ -8514,7 +8541,7 @@
       <c r="C277" s="1"/>
       <c r="D277" s="2"/>
       <c r="E277" s="3" t="s">
-        <v>616</v>
+        <v>610</v>
       </c>
       <c r="F277" s="4">
         <v>42013</v>
@@ -8530,7 +8557,7 @@
       <c r="C278" s="1"/>
       <c r="D278" s="2"/>
       <c r="E278" s="3" t="s">
-        <v>617</v>
+        <v>611</v>
       </c>
       <c r="F278" s="4">
         <v>42013</v>
@@ -8546,7 +8573,7 @@
       <c r="C279" s="1"/>
       <c r="D279" s="2"/>
       <c r="E279" s="3" t="s">
-        <v>618</v>
+        <v>612</v>
       </c>
       <c r="F279" s="4">
         <v>42013</v>
@@ -8562,7 +8589,7 @@
       <c r="C280" s="1"/>
       <c r="D280" s="2"/>
       <c r="E280" s="3" t="s">
-        <v>619</v>
+        <v>613</v>
       </c>
       <c r="F280" s="4">
         <v>42013</v>
@@ -8578,7 +8605,7 @@
       <c r="C281" s="1"/>
       <c r="D281" s="2"/>
       <c r="E281" s="3" t="s">
-        <v>620</v>
+        <v>614</v>
       </c>
       <c r="F281" s="4">
         <v>42013</v>
@@ -8594,7 +8621,7 @@
       <c r="C282" s="1"/>
       <c r="D282" s="2"/>
       <c r="E282" s="3" t="s">
-        <v>621</v>
+        <v>615</v>
       </c>
       <c r="F282" s="4">
         <v>42013</v>
@@ -8610,7 +8637,7 @@
       <c r="C283" s="1"/>
       <c r="D283" s="2"/>
       <c r="E283" s="3" t="s">
-        <v>622</v>
+        <v>616</v>
       </c>
       <c r="F283" s="4">
         <v>42013</v>
@@ -8626,7 +8653,7 @@
       <c r="C284" s="1"/>
       <c r="D284" s="2"/>
       <c r="E284" s="3" t="s">
-        <v>623</v>
+        <v>617</v>
       </c>
       <c r="F284" s="4">
         <v>42013</v>
@@ -8642,7 +8669,7 @@
       <c r="C285" s="1"/>
       <c r="D285" s="2"/>
       <c r="E285" s="3" t="s">
-        <v>624</v>
+        <v>618</v>
       </c>
       <c r="F285" s="4">
         <v>42013</v>
@@ -8658,7 +8685,7 @@
       <c r="C286" s="1"/>
       <c r="D286" s="2"/>
       <c r="E286" s="3" t="s">
-        <v>625</v>
+        <v>619</v>
       </c>
       <c r="F286" s="4">
         <v>42013</v>
@@ -8674,7 +8701,7 @@
       <c r="C287" s="1"/>
       <c r="D287" s="2"/>
       <c r="E287" s="3" t="s">
-        <v>626</v>
+        <v>620</v>
       </c>
       <c r="F287" s="4">
         <v>42013</v>
@@ -8690,7 +8717,7 @@
       <c r="C288" s="1"/>
       <c r="D288" s="2"/>
       <c r="E288" s="3" t="s">
-        <v>627</v>
+        <v>621</v>
       </c>
       <c r="F288" s="4">
         <v>42013</v>
@@ -8706,7 +8733,7 @@
       <c r="C289" s="1"/>
       <c r="D289" s="2"/>
       <c r="E289" s="3" t="s">
-        <v>628</v>
+        <v>622</v>
       </c>
       <c r="F289" s="4">
         <v>42013</v>
@@ -8722,7 +8749,7 @@
       <c r="C290" s="1"/>
       <c r="D290" s="2"/>
       <c r="E290" s="3" t="s">
-        <v>629</v>
+        <v>623</v>
       </c>
       <c r="F290" s="4">
         <v>42013</v>
@@ -8738,7 +8765,7 @@
       <c r="C291" s="1"/>
       <c r="D291" s="2"/>
       <c r="E291" s="3" t="s">
-        <v>630</v>
+        <v>624</v>
       </c>
       <c r="F291" s="4">
         <v>42013</v>
@@ -8754,7 +8781,7 @@
       <c r="C292" s="1"/>
       <c r="D292" s="2"/>
       <c r="E292" s="3" t="s">
-        <v>631</v>
+        <v>625</v>
       </c>
       <c r="F292" s="4">
         <v>42013</v>
@@ -8770,7 +8797,7 @@
       <c r="C293" s="1"/>
       <c r="D293" s="2"/>
       <c r="E293" s="3" t="s">
-        <v>632</v>
+        <v>626</v>
       </c>
       <c r="F293" s="4">
         <v>42013</v>
@@ -8786,7 +8813,7 @@
       <c r="C294" s="1"/>
       <c r="D294" s="2"/>
       <c r="E294" s="3" t="s">
-        <v>633</v>
+        <v>627</v>
       </c>
       <c r="F294" s="4">
         <v>42013</v>
@@ -8802,7 +8829,7 @@
       <c r="C295" s="1"/>
       <c r="D295" s="2"/>
       <c r="E295" s="3" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="F295" s="4">
         <v>42013</v>
@@ -8818,7 +8845,7 @@
       <c r="C296" s="1"/>
       <c r="D296" s="2"/>
       <c r="E296" s="3" t="s">
-        <v>635</v>
+        <v>629</v>
       </c>
       <c r="F296" s="4">
         <v>42013</v>
@@ -8834,7 +8861,7 @@
       <c r="C297" s="1"/>
       <c r="D297" s="2"/>
       <c r="E297" s="3" t="s">
-        <v>636</v>
+        <v>630</v>
       </c>
       <c r="F297" s="4">
         <v>42013</v>
@@ -8850,7 +8877,7 @@
       <c r="C298" s="1"/>
       <c r="D298" s="2"/>
       <c r="E298" s="3" t="s">
-        <v>637</v>
+        <v>631</v>
       </c>
       <c r="F298" s="4">
         <v>42013</v>
@@ -8866,7 +8893,7 @@
       <c r="C299" s="1"/>
       <c r="D299" s="2"/>
       <c r="E299" s="3" t="s">
-        <v>638</v>
+        <v>632</v>
       </c>
       <c r="F299" s="4">
         <v>42013</v>
@@ -8882,7 +8909,7 @@
       <c r="C300" s="1"/>
       <c r="D300" s="2"/>
       <c r="E300" s="3" t="s">
-        <v>639</v>
+        <v>633</v>
       </c>
       <c r="F300" s="4">
         <v>42013</v>
@@ -8898,7 +8925,7 @@
       <c r="C301" s="1"/>
       <c r="D301" s="2"/>
       <c r="E301" s="3" t="s">
-        <v>640</v>
+        <v>634</v>
       </c>
       <c r="F301" s="4">
         <v>42013</v>
@@ -8914,7 +8941,7 @@
       <c r="C302" s="1"/>
       <c r="D302" s="2"/>
       <c r="E302" s="3" t="s">
-        <v>641</v>
+        <v>635</v>
       </c>
       <c r="F302" s="4">
         <v>42013</v>
@@ -8930,7 +8957,7 @@
       <c r="C303" s="1"/>
       <c r="D303" s="2"/>
       <c r="E303" s="3" t="s">
-        <v>642</v>
+        <v>636</v>
       </c>
       <c r="F303" s="4">
         <v>42013</v>
@@ -8946,7 +8973,7 @@
       <c r="C304" s="1"/>
       <c r="D304" s="2"/>
       <c r="E304" s="3" t="s">
-        <v>643</v>
+        <v>637</v>
       </c>
       <c r="F304" s="4">
         <v>42013</v>
@@ -8962,7 +8989,7 @@
       <c r="C305" s="1"/>
       <c r="D305" s="2"/>
       <c r="E305" s="3" t="s">
-        <v>644</v>
+        <v>638</v>
       </c>
       <c r="F305" s="4">
         <v>42013</v>
@@ -8978,7 +9005,7 @@
       <c r="C306" s="1"/>
       <c r="D306" s="2"/>
       <c r="E306" s="3" t="s">
-        <v>645</v>
+        <v>639</v>
       </c>
       <c r="F306" s="4">
         <v>42013</v>
@@ -8994,7 +9021,7 @@
       <c r="C307" s="1"/>
       <c r="D307" s="2"/>
       <c r="E307" s="3" t="s">
-        <v>646</v>
+        <v>640</v>
       </c>
       <c r="F307" s="4">
         <v>42013</v>
@@ -9010,7 +9037,7 @@
       <c r="C308" s="1"/>
       <c r="D308" s="2"/>
       <c r="E308" s="3" t="s">
-        <v>647</v>
+        <v>641</v>
       </c>
       <c r="F308" s="4">
         <v>42013</v>
@@ -9026,7 +9053,7 @@
       <c r="C309" s="1"/>
       <c r="D309" s="2"/>
       <c r="E309" s="3" t="s">
-        <v>648</v>
+        <v>642</v>
       </c>
       <c r="F309" s="4">
         <v>42013</v>
@@ -9042,7 +9069,7 @@
       <c r="C310" s="1"/>
       <c r="D310" s="2"/>
       <c r="E310" s="3" t="s">
-        <v>649</v>
+        <v>643</v>
       </c>
       <c r="F310" s="4">
         <v>42013</v>
@@ -9058,7 +9085,7 @@
       <c r="C311" s="1"/>
       <c r="D311" s="2"/>
       <c r="E311" s="3" t="s">
-        <v>650</v>
+        <v>644</v>
       </c>
       <c r="F311" s="4">
         <v>42013</v>
@@ -9074,7 +9101,7 @@
       <c r="C312" s="1"/>
       <c r="D312" s="2"/>
       <c r="E312" s="3" t="s">
-        <v>651</v>
+        <v>645</v>
       </c>
       <c r="F312" s="4">
         <v>42013</v>
@@ -9090,7 +9117,7 @@
       <c r="C313" s="1"/>
       <c r="D313" s="2"/>
       <c r="E313" s="3" t="s">
-        <v>652</v>
+        <v>646</v>
       </c>
       <c r="F313" s="4">
         <v>42013</v>
@@ -9106,7 +9133,7 @@
       <c r="C314" s="1"/>
       <c r="D314" s="2"/>
       <c r="E314" s="3" t="s">
-        <v>653</v>
+        <v>647</v>
       </c>
       <c r="F314" s="4">
         <v>42013</v>
@@ -9122,7 +9149,7 @@
       <c r="C315" s="1"/>
       <c r="D315" s="2"/>
       <c r="E315" s="3" t="s">
-        <v>654</v>
+        <v>648</v>
       </c>
       <c r="F315" s="4">
         <v>42013</v>
@@ -9138,7 +9165,7 @@
       <c r="C316" s="1"/>
       <c r="D316" s="2"/>
       <c r="E316" s="3" t="s">
-        <v>655</v>
+        <v>649</v>
       </c>
       <c r="F316" s="4">
         <v>42013</v>
@@ -9154,7 +9181,7 @@
       <c r="C317" s="1"/>
       <c r="D317" s="2"/>
       <c r="E317" s="3" t="s">
-        <v>656</v>
+        <v>650</v>
       </c>
       <c r="F317" s="4">
         <v>42013</v>
@@ -9170,7 +9197,7 @@
       <c r="C318" s="1"/>
       <c r="D318" s="2"/>
       <c r="E318" s="3" t="s">
-        <v>657</v>
+        <v>651</v>
       </c>
       <c r="F318" s="4">
         <v>42013</v>
@@ -9186,7 +9213,7 @@
       <c r="C319" s="1"/>
       <c r="D319" s="2"/>
       <c r="E319" s="3" t="s">
-        <v>658</v>
+        <v>652</v>
       </c>
       <c r="F319" s="4">
         <v>42013</v>
@@ -9202,7 +9229,7 @@
       <c r="C320" s="1"/>
       <c r="D320" s="2"/>
       <c r="E320" s="3" t="s">
-        <v>659</v>
+        <v>653</v>
       </c>
       <c r="F320" s="4">
         <v>42013</v>
@@ -9218,7 +9245,7 @@
       <c r="C321" s="1"/>
       <c r="D321" s="2"/>
       <c r="E321" s="3" t="s">
-        <v>660</v>
+        <v>654</v>
       </c>
       <c r="F321" s="4">
         <v>42013</v>
@@ -9234,7 +9261,7 @@
       <c r="C322" s="1"/>
       <c r="D322" s="2"/>
       <c r="E322" s="3" t="s">
-        <v>661</v>
+        <v>655</v>
       </c>
       <c r="F322" s="4">
         <v>42013</v>
@@ -9250,7 +9277,7 @@
       <c r="C323" s="1"/>
       <c r="D323" s="2"/>
       <c r="E323" s="3" t="s">
-        <v>662</v>
+        <v>656</v>
       </c>
       <c r="F323" s="4">
         <v>42013</v>
@@ -9266,7 +9293,7 @@
       <c r="C324" s="1"/>
       <c r="D324" s="2"/>
       <c r="E324" s="3" t="s">
-        <v>663</v>
+        <v>657</v>
       </c>
       <c r="F324" s="4">
         <v>42013</v>
@@ -9282,7 +9309,7 @@
       <c r="C325" s="1"/>
       <c r="D325" s="2"/>
       <c r="E325" s="3" t="s">
-        <v>664</v>
+        <v>658</v>
       </c>
       <c r="F325" s="4">
         <v>42013</v>
@@ -9298,7 +9325,7 @@
       <c r="C326" s="1"/>
       <c r="D326" s="2"/>
       <c r="E326" s="3" t="s">
-        <v>665</v>
+        <v>659</v>
       </c>
       <c r="F326" s="4">
         <v>42013</v>
@@ -9314,7 +9341,7 @@
       <c r="C327" s="1"/>
       <c r="D327" s="2"/>
       <c r="E327" s="3" t="s">
-        <v>666</v>
+        <v>660</v>
       </c>
       <c r="F327" s="4">
         <v>42013</v>
@@ -9330,7 +9357,7 @@
       <c r="C328" s="1"/>
       <c r="D328" s="2"/>
       <c r="E328" s="3" t="s">
-        <v>667</v>
+        <v>661</v>
       </c>
       <c r="F328" s="4">
         <v>42013</v>
@@ -9346,7 +9373,7 @@
       <c r="C329" s="1"/>
       <c r="D329" s="2"/>
       <c r="E329" s="3" t="s">
-        <v>668</v>
+        <v>662</v>
       </c>
       <c r="F329" s="4">
         <v>42013</v>
@@ -9362,7 +9389,7 @@
       <c r="C330" s="1"/>
       <c r="D330" s="2"/>
       <c r="E330" s="3" t="s">
-        <v>669</v>
+        <v>663</v>
       </c>
       <c r="F330" s="4">
         <v>42013</v>
@@ -9378,7 +9405,7 @@
       <c r="C331" s="1"/>
       <c r="D331" s="2"/>
       <c r="E331" s="3" t="s">
-        <v>670</v>
+        <v>664</v>
       </c>
       <c r="F331" s="4">
         <v>42013</v>
@@ -9394,7 +9421,7 @@
       <c r="C332" s="1"/>
       <c r="D332" s="2"/>
       <c r="E332" s="3" t="s">
-        <v>671</v>
+        <v>665</v>
       </c>
       <c r="F332" s="4">
         <v>42013</v>
@@ -9410,7 +9437,7 @@
       <c r="C333" s="1"/>
       <c r="D333" s="2"/>
       <c r="E333" s="3" t="s">
-        <v>672</v>
+        <v>666</v>
       </c>
       <c r="F333" s="4">
         <v>42013</v>
@@ -9426,7 +9453,7 @@
       <c r="C334" s="1"/>
       <c r="D334" s="2"/>
       <c r="E334" s="3" t="s">
-        <v>673</v>
+        <v>667</v>
       </c>
       <c r="F334" s="4">
         <v>42013</v>
@@ -9442,7 +9469,7 @@
       <c r="C335" s="1"/>
       <c r="D335" s="2"/>
       <c r="E335" s="3" t="s">
-        <v>674</v>
+        <v>668</v>
       </c>
       <c r="F335" s="4">
         <v>42013</v>
@@ -9458,7 +9485,7 @@
       <c r="C336" s="1"/>
       <c r="D336" s="2"/>
       <c r="E336" s="3" t="s">
-        <v>675</v>
+        <v>669</v>
       </c>
       <c r="F336" s="4">
         <v>42013</v>
@@ -9474,7 +9501,7 @@
       <c r="C337" s="1"/>
       <c r="D337" s="2"/>
       <c r="E337" s="3" t="s">
-        <v>676</v>
+        <v>670</v>
       </c>
       <c r="F337" s="4">
         <v>42013</v>
@@ -9490,7 +9517,7 @@
       <c r="C338" s="1"/>
       <c r="D338" s="2"/>
       <c r="E338" s="3" t="s">
-        <v>677</v>
+        <v>671</v>
       </c>
       <c r="F338" s="4">
         <v>42013</v>
@@ -9506,7 +9533,7 @@
       <c r="C339" s="1"/>
       <c r="D339" s="2"/>
       <c r="E339" s="3" t="s">
-        <v>678</v>
+        <v>672</v>
       </c>
       <c r="F339" s="4">
         <v>42013</v>
@@ -9522,7 +9549,7 @@
       <c r="C340" s="1"/>
       <c r="D340" s="2"/>
       <c r="E340" s="3" t="s">
-        <v>679</v>
+        <v>673</v>
       </c>
       <c r="F340" s="4">
         <v>42013</v>
@@ -9538,7 +9565,7 @@
       <c r="C341" s="1"/>
       <c r="D341" s="2"/>
       <c r="E341" s="3" t="s">
-        <v>680</v>
+        <v>674</v>
       </c>
       <c r="F341" s="4">
         <v>42013</v>
@@ -9554,7 +9581,7 @@
       <c r="C342" s="1"/>
       <c r="D342" s="2"/>
       <c r="E342" s="3" t="s">
-        <v>681</v>
+        <v>675</v>
       </c>
       <c r="F342" s="4">
         <v>42013</v>
@@ -9570,7 +9597,7 @@
       <c r="C343" s="1"/>
       <c r="D343" s="2"/>
       <c r="E343" s="3" t="s">
-        <v>682</v>
+        <v>676</v>
       </c>
       <c r="F343" s="4">
         <v>42013</v>
@@ -9586,7 +9613,7 @@
       <c r="C344" s="1"/>
       <c r="D344" s="2"/>
       <c r="E344" s="3" t="s">
-        <v>683</v>
+        <v>677</v>
       </c>
       <c r="F344" s="4">
         <v>42013</v>
@@ -9594,7 +9621,7 @@
     </row>
     <row r="345" spans="1:6">
       <c r="A345" s="1" t="s">
-        <v>684</v>
+        <v>678</v>
       </c>
       <c r="B345" s="1" t="s">
         <v>1</v>
@@ -9602,7 +9629,7 @@
       <c r="C345" s="1"/>
       <c r="D345" s="2"/>
       <c r="E345" s="3" t="s">
-        <v>687</v>
+        <v>681</v>
       </c>
       <c r="F345" s="4">
         <v>42013</v>
@@ -9610,7 +9637,7 @@
     </row>
     <row r="346" spans="1:6">
       <c r="A346" s="1" t="s">
-        <v>685</v>
+        <v>679</v>
       </c>
       <c r="B346" s="1" t="s">
         <v>1</v>
@@ -9618,7 +9645,7 @@
       <c r="C346" s="1"/>
       <c r="D346" s="2"/>
       <c r="E346" s="3" t="s">
-        <v>688</v>
+        <v>682</v>
       </c>
       <c r="F346" s="4">
         <v>42013</v>
@@ -9626,7 +9653,7 @@
     </row>
     <row r="347" spans="1:6">
       <c r="A347" s="1" t="s">
-        <v>686</v>
+        <v>680</v>
       </c>
       <c r="B347" s="1" t="s">
         <v>1</v>
@@ -9634,7 +9661,7 @@
       <c r="C347" s="1"/>
       <c r="D347" s="2"/>
       <c r="E347" s="3" t="s">
-        <v>689</v>
+        <v>683</v>
       </c>
       <c r="F347" s="4">
         <v>42013</v>
@@ -9642,7 +9669,7 @@
     </row>
     <row r="348" spans="1:6">
       <c r="A348" s="1" t="s">
-        <v>690</v>
+        <v>684</v>
       </c>
       <c r="B348" s="1" t="s">
         <v>1</v>
@@ -9650,7 +9677,7 @@
       <c r="C348" s="1"/>
       <c r="D348" s="2"/>
       <c r="E348" s="5" t="s">
-        <v>697</v>
+        <v>691</v>
       </c>
       <c r="F348" s="4">
         <v>42013</v>
@@ -9658,7 +9685,7 @@
     </row>
     <row r="349" spans="1:6">
       <c r="A349" s="1" t="s">
-        <v>691</v>
+        <v>685</v>
       </c>
       <c r="B349" s="1" t="s">
         <v>1</v>
@@ -9666,7 +9693,7 @@
       <c r="C349" s="1"/>
       <c r="D349" s="2"/>
       <c r="E349" s="5" t="s">
-        <v>698</v>
+        <v>692</v>
       </c>
       <c r="F349" s="4">
         <v>42013</v>
@@ -9674,7 +9701,7 @@
     </row>
     <row r="350" spans="1:6">
       <c r="A350" s="1" t="s">
-        <v>692</v>
+        <v>686</v>
       </c>
       <c r="B350" s="1" t="s">
         <v>1</v>
@@ -9682,7 +9709,7 @@
       <c r="C350" s="1"/>
       <c r="D350" s="2"/>
       <c r="E350" s="5" t="s">
-        <v>699</v>
+        <v>693</v>
       </c>
       <c r="F350" s="4">
         <v>42013</v>
@@ -9690,7 +9717,7 @@
     </row>
     <row r="351" spans="1:6">
       <c r="A351" s="1" t="s">
-        <v>693</v>
+        <v>687</v>
       </c>
       <c r="B351" s="1" t="s">
         <v>1</v>
@@ -9698,7 +9725,7 @@
       <c r="C351" s="1"/>
       <c r="D351" s="2"/>
       <c r="E351" s="5" t="s">
-        <v>696</v>
+        <v>690</v>
       </c>
       <c r="F351" s="4">
         <v>42013</v>
@@ -9706,7 +9733,7 @@
     </row>
     <row r="352" spans="1:6">
       <c r="A352" s="1" t="s">
-        <v>694</v>
+        <v>688</v>
       </c>
       <c r="B352" s="1" t="s">
         <v>1</v>
@@ -9714,9 +9741,25 @@
       <c r="C352" s="1"/>
       <c r="D352" s="2"/>
       <c r="E352" s="5" t="s">
-        <v>695</v>
+        <v>689</v>
       </c>
       <c r="F352" s="4">
+        <v>42013</v>
+      </c>
+    </row>
+    <row r="353" spans="1:6">
+      <c r="A353" s="1" t="s">
+        <v>702</v>
+      </c>
+      <c r="B353" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C353" s="1"/>
+      <c r="D353" s="2"/>
+      <c r="E353" s="3" t="s">
+        <v>703</v>
+      </c>
+      <c r="F353" s="4">
         <v>42013</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added product placement v5
</commit_message>
<xml_diff>
--- a/publication/part1000/CR00011/CR11_WG_Numbers_table.xlsx
+++ b/publication/part1000/CR00011/CR11_WG_Numbers_table.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="27820" windowHeight="17460" tabRatio="500"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1060" uniqueCount="705">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1063" uniqueCount="707">
   <si>
     <t>N8573</t>
   </si>
@@ -2134,6 +2134,12 @@
   </si>
   <si>
     <t>ISO 10303-1819  ed  2 tessellated_geometry MIM EXPRESS</t>
+  </si>
+  <si>
+    <t>N9124</t>
+  </si>
+  <si>
+    <t>ISO 10303-1343 ed 5 product_placement Document</t>
   </si>
 </sst>
 </file>
@@ -2203,8 +2209,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="787">
+  <cellStyleXfs count="791">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3008,7 +3018,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="787">
+  <cellStyles count="791">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
@@ -3402,6 +3412,8 @@
     <cellStyle name="Lien hypertexte" xfId="781" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="783" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="785" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="787" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="789" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
@@ -3795,6 +3807,8 @@
     <cellStyle name="Lien hypertexte visité" xfId="782" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="784" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="786" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="788" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="790" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4124,10 +4138,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G353"/>
+  <dimension ref="A1:G354"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
-      <selection activeCell="E134" sqref="E134"/>
+    <sheetView tabSelected="1" topLeftCell="A337" workbookViewId="0">
+      <selection activeCell="G356" sqref="G356"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -9789,6 +9803,22 @@
         <v>42013</v>
       </c>
     </row>
+    <row r="354" spans="1:6">
+      <c r="A354" s="1" t="s">
+        <v>705</v>
+      </c>
+      <c r="B354" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C354" s="1"/>
+      <c r="D354" s="2"/>
+      <c r="E354" s="3" t="s">
+        <v>706</v>
+      </c>
+      <c r="F354" s="4">
+        <v>42013</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>